<commit_message>
20 anniversary plan doc pre-publish
</commit_message>
<xml_diff>
--- a/class70/contacts.xlsx
+++ b/class70/contacts.xlsx
@@ -398,15 +398,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>田斌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>夏志毅</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>万国振</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>田兵</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1340,7 +1340,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>18273360816</v>
@@ -1369,6 +1369,9 @@
       <c r="A3" t="s">
         <v>98</v>
       </c>
+      <c r="B3">
+        <v>15873338161</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -1382,6 +1385,9 @@
       <c r="A5" t="s">
         <v>100</v>
       </c>
+      <c r="B5">
+        <v>13337334566</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -1395,6 +1401,9 @@
       <c r="A7" t="s">
         <v>102</v>
       </c>
+      <c r="B7">
+        <v>13037330613</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -1403,17 +1412,26 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="B9">
+        <v>18907337711</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>104</v>
       </c>
+      <c r="B10">
+        <v>13077088869</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="B11">
+        <v>13037338887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>